<commit_message>
added Reggio Calabria to the table and map
</commit_message>
<xml_diff>
--- a/Italy.xlsx
+++ b/Italy.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -144,7 +144,7 @@
     <t>Relaxing in the hot Rome summer admiring the beautiful Vittorio Emanuele Monument.</t>
   </si>
   <si>
-    <t>https://media-cdn.tripadvisor.com/media/photo-s/14/60/3b/32/fontana-di-trevi.jpg</t>
+    <t>https://news.artnet.com/app/news-upload/2015/07/Fontana-di-Trevi.png</t>
   </si>
   <si>
     <t>The beautiful Fontana di Trevi!!</t>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>Il Catello di Palizzi</t>
+  </si>
+  <si>
+    <t>Reggio di Calabria</t>
+  </si>
+  <si>
+    <t>http://www.classicult.it/wp-content/uploads/2019/04/PHOTO-2018-03-16-21-23-20-1024x683.jpg</t>
+  </si>
+  <si>
+    <t>The capital of the Calabrese Province. Here ‘L’Arenna dello Stretto’ in which you can find the statue of ‘Athena Promachos’ that protects the city.</t>
+  </si>
+  <si>
+    <t>rabarama.JPG</t>
+  </si>
+  <si>
+    <t>This modern art is in the main road of this beautiful city. It was designed by the famous Italian artist Paola Rabarama.</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/d/d1/Il_prospetto_principale_del_duomo.jpg</t>
+  </si>
+  <si>
+    <t>Reggio di Calabria’s Cathedral</t>
   </si>
 </sst>
 </file>
@@ -1865,15 +1886,33 @@
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+      <c r="A6" t="s" s="25">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s" s="25">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s" s="25">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s" s="25">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s" s="25">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s" s="25">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s" s="25">
+        <v>51</v>
+      </c>
+      <c r="H6" s="26">
+        <v>38.106266</v>
+      </c>
+      <c r="I6" s="26">
+        <v>15.647941</v>
+      </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="29"/>

</xml_diff>